<commit_message>
Fixed delta AIC Tables
</commit_message>
<xml_diff>
--- a/Tables/Global_delta_AIC.xlsx
+++ b/Tables/Global_delta_AIC.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel_anstett/Dropbox/a Papers/Rapid_drought/Paper 3/climate_lag/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE7839D-9049-3246-BFBA-77FF171D6F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD2BF62-6576-C346-8FFF-F5864E114627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global_delta_AIC_DF" sheetId="1" r:id="rId1"/>
+    <sheet name="Old" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
   <si>
     <t>SPEI</t>
   </si>
@@ -59,7 +60,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -194,8 +195,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +395,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -562,25 +584,33 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -938,23 +968,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -968,180 +995,93 @@
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5">
-        <v>22.946818296979501</v>
+        <v>19.514364959839401</v>
       </c>
       <c r="C3" s="5">
-        <v>28.274938075595902</v>
-      </c>
-      <c r="D3" s="5">
-        <v>3.4324533371400299</v>
+        <v>84.170679522758306</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
       </c>
       <c r="E3" s="5">
-        <v>87.603132859898295</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8">
-        <v>19.514364959839401</v>
-      </c>
-      <c r="I3" s="8">
         <v>24.842484738455799</v>
       </c>
-      <c r="J3" s="9">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>84.170679522758306</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="5">
-        <v>31.035028293812498</v>
+        <v>27.602574956672498</v>
       </c>
       <c r="C4" s="5">
-        <v>32.246274834273201</v>
-      </c>
-      <c r="D4" s="5">
-        <v>5.9909307632660802</v>
+        <v>82.808858166605205</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2.5584774261260499</v>
       </c>
       <c r="E4" s="5">
-        <v>86.241311503745194</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4" s="8">
-        <v>27.602574956672498</v>
-      </c>
-      <c r="I4" s="8">
         <v>28.813821497133201</v>
       </c>
-      <c r="J4" s="8">
-        <v>2.5584774261260499</v>
-      </c>
-      <c r="K4" s="8">
-        <v>82.808858166605205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="5">
-        <v>26.8351548320388</v>
+        <v>23.4027014948988</v>
       </c>
       <c r="C5" s="5">
-        <v>31.1957448115791</v>
-      </c>
-      <c r="D5" s="5">
-        <v>5.0750563486944902</v>
+        <v>77.716130751578007</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1.6426030115544601</v>
       </c>
       <c r="E5" s="5">
-        <v>81.148584088718096</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5" s="8">
-        <v>23.4027014948988</v>
-      </c>
-      <c r="I5" s="8">
         <v>27.763291474439001</v>
       </c>
-      <c r="J5" s="9">
-        <v>1.6426030115544601</v>
-      </c>
-      <c r="K5" s="8">
-        <v>77.716130751578007</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5">
-        <v>35.8190415773133</v>
+        <v>32.386588240173303</v>
       </c>
       <c r="C6" s="5">
-        <v>30.219026452490699</v>
+        <v>91.957544288601596</v>
       </c>
       <c r="D6" s="5">
-        <v>6.8878214057076503</v>
+        <v>11.773134234616</v>
       </c>
       <c r="E6" s="5">
-        <v>95.389997625741699</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6" s="8">
-        <v>32.386588240173303</v>
-      </c>
-      <c r="I6" s="8">
         <v>35.104339353987598</v>
       </c>
-      <c r="J6" s="8">
-        <v>11.773134234616</v>
-      </c>
-      <c r="K6" s="8">
-        <v>91.957544288601596</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6">
-        <v>34.686540128968801</v>
-      </c>
-      <c r="C7" s="6">
-        <v>29.7355596317575</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>95.157708879276498</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7" s="8">
+      <c r="B7" s="5">
         <v>31.254086791828701</v>
       </c>
-      <c r="I7" s="8">
+      <c r="C7" s="5">
+        <v>91.725255542136395</v>
+      </c>
+      <c r="D7" s="5">
+        <v>9.7508941261730797</v>
+      </c>
+      <c r="E7" s="5">
         <v>39.486453850739103</v>
       </c>
-      <c r="J7" s="8">
-        <v>9.7508941261730797</v>
-      </c>
-      <c r="K7" s="8">
-        <v>91.725255542136395</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1149,11 +1089,8 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="H9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>0</v>
@@ -1167,180 +1104,333 @@
       <c r="E10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="5">
-        <v>34.800824524307203</v>
+        <v>30.041165323862501</v>
       </c>
       <c r="C11" s="5">
-        <v>37.522239279620401</v>
+        <v>80.384231324711394</v>
       </c>
       <c r="D11" s="5">
-        <v>9.9395854942158604</v>
+        <v>5.1799262937711301</v>
       </c>
       <c r="E11" s="5">
-        <v>85.143890525156195</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" s="8">
-        <v>30.041165323862501</v>
-      </c>
-      <c r="I11" s="8">
         <v>32.762580079175699</v>
       </c>
-      <c r="J11" s="8">
-        <v>5.1799262937711301</v>
-      </c>
-      <c r="K11" s="8">
-        <v>80.384231324711394</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="5">
-        <v>31.8436805832498</v>
+        <v>27.084021382805101</v>
       </c>
       <c r="C12" s="5">
-        <v>33.789556131534503</v>
-      </c>
-      <c r="D12" s="5">
-        <v>5.55049903071267</v>
+        <v>71.914550964636902</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.79083983026794202</v>
       </c>
       <c r="E12" s="5">
-        <v>76.674210165081604</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12" s="8">
-        <v>27.084021382805101</v>
-      </c>
-      <c r="I12" s="8">
         <v>29.029896931089802</v>
       </c>
-      <c r="J12" s="9">
-        <v>0.79083983026794202</v>
-      </c>
-      <c r="K12" s="8">
-        <v>71.914550964636902</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="5">
-        <v>35.530062835015997</v>
+        <v>30.770403634571299</v>
       </c>
       <c r="C13" s="5">
-        <v>30.080306252584698</v>
-      </c>
-      <c r="D13" s="5">
-        <v>4.7596592004447302</v>
+        <v>78.823208049296198</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0</v>
       </c>
       <c r="E13" s="5">
-        <v>83.582867249741</v>
-      </c>
-      <c r="G13">
-        <v>3</v>
-      </c>
-      <c r="H13" s="8">
-        <v>30.770403634571299</v>
-      </c>
-      <c r="I13" s="8">
         <v>25.32064705214</v>
       </c>
-      <c r="J13" s="9">
-        <v>0</v>
-      </c>
-      <c r="K13" s="8">
-        <v>78.823208049296198</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="5">
-        <v>42.074063981308399</v>
+        <v>37.314404780863697</v>
       </c>
       <c r="C14" s="5">
-        <v>37.952240730901401</v>
+        <v>84.631661195657202</v>
       </c>
       <c r="D14" s="5">
-        <v>2.7634184981216099</v>
+        <v>6.3215254643910201</v>
       </c>
       <c r="E14" s="5">
-        <v>89.391320396101904</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
-      <c r="H14" s="8">
-        <v>37.314404780863697</v>
-      </c>
-      <c r="I14" s="8">
         <v>41.510347758991003</v>
       </c>
-      <c r="J14" s="8">
-        <v>6.3215254643910201</v>
-      </c>
-      <c r="K14" s="8">
-        <v>84.631661195657202</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="6">
-        <v>45.553647374963496</v>
-      </c>
-      <c r="C15" s="6">
-        <v>36.195362397094897</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6">
-        <v>91.430487107722001</v>
-      </c>
-      <c r="G15">
-        <v>5</v>
-      </c>
-      <c r="H15" s="8">
+      <c r="B15" s="5">
         <v>40.793988174518702</v>
       </c>
-      <c r="I15" s="8">
+      <c r="C15" s="5">
+        <v>86.6708279072773</v>
+      </c>
+      <c r="D15" s="5">
+        <v>8.4236882717741501</v>
+      </c>
+      <c r="E15" s="5">
         <v>44.619050432913397</v>
-      </c>
-      <c r="J15" s="8">
-        <v>8.4236882717741501</v>
-      </c>
-      <c r="K15" s="8">
-        <v>86.6708279072773</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6ECB2D-AB64-F545-A947-2047CCDBB078}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="12">
+        <v>22.95</v>
+      </c>
+      <c r="C3" s="12">
+        <v>28.27</v>
+      </c>
+      <c r="D3" s="12">
+        <v>3.43</v>
+      </c>
+      <c r="E3" s="12">
+        <v>87.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="12">
+        <v>31.04</v>
+      </c>
+      <c r="C4" s="12">
+        <v>32.25</v>
+      </c>
+      <c r="D4" s="12">
+        <v>5.99</v>
+      </c>
+      <c r="E4" s="12">
+        <v>86.24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12">
+        <v>26.84</v>
+      </c>
+      <c r="C5" s="12">
+        <v>31.2</v>
+      </c>
+      <c r="D5" s="12">
+        <v>5.08</v>
+      </c>
+      <c r="E5" s="12">
+        <v>81.150000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="12">
+        <v>35.82</v>
+      </c>
+      <c r="C6" s="12">
+        <v>30.22</v>
+      </c>
+      <c r="D6" s="12">
+        <v>6.89</v>
+      </c>
+      <c r="E6" s="12">
+        <v>95.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="14">
+        <v>34.69</v>
+      </c>
+      <c r="C7" s="14">
+        <v>29.74</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0</v>
+      </c>
+      <c r="E7" s="14">
+        <v>95.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="12">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="C11" s="12">
+        <v>37.520000000000003</v>
+      </c>
+      <c r="D11" s="12">
+        <v>9.94</v>
+      </c>
+      <c r="E11" s="12">
+        <v>85.14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12">
+        <v>31.84</v>
+      </c>
+      <c r="C12" s="12">
+        <v>33.79</v>
+      </c>
+      <c r="D12" s="12">
+        <v>5.55</v>
+      </c>
+      <c r="E12" s="12">
+        <v>76.67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="12">
+        <v>35.53</v>
+      </c>
+      <c r="C13" s="12">
+        <v>30.08</v>
+      </c>
+      <c r="D13" s="12">
+        <v>4.76</v>
+      </c>
+      <c r="E13" s="12">
+        <v>83.58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="12">
+        <v>42.07</v>
+      </c>
+      <c r="C14" s="12">
+        <v>37.950000000000003</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2.76</v>
+      </c>
+      <c r="E14" s="12">
+        <v>89.39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="14">
+        <v>45.55</v>
+      </c>
+      <c r="C15" s="14">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="14">
+        <v>91.43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>